<commit_message>
admin can remove staff, make middlename optional
</commit_message>
<xml_diff>
--- a/src/tests/integration/__tests__/testFiles/validBranches.xlsx
+++ b/src/tests/integration/__tests__/testFiles/validBranches.xlsx
@@ -70,12 +70,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -88,16 +94,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -114,13 +120,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -140,6 +146,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -278,13 +285,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -383,10 +384,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -641,13 +642,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -960,10 +955,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1232,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>1234</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s" s="2">
         <v>1</v>
@@ -1245,7 +1240,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>4321</v>
+        <v>432</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>1</v>
@@ -1258,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>8765</v>
+        <v>876</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>1</v>
@@ -1271,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>5434</v>
+        <v>543</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>1</v>
@@ -1284,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>8097</v>
+        <v>809</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>1</v>
@@ -1297,7 +1292,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>1479</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s" s="2">
         <v>1</v>
@@ -1310,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <v>9874</v>
+        <v>987</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>1</v>
@@ -1323,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>3092</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s" s="2">
         <v>1</v>
@@ -1336,7 +1331,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>2947</v>
+        <v>294</v>
       </c>
       <c r="C9" t="s" s="2">
         <v>1</v>
@@ -1349,7 +1344,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>9067</v>
+        <v>907</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>1</v>

</xml_diff>